<commit_message>
Better scenario for google meet
</commit_message>
<xml_diff>
--- a/entwicklung-sicherer-software-systeme/exercise-1/risks.xlsx
+++ b/entwicklung-sicherer-software-systeme/exercise-1/risks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="137">
   <si>
     <t>Severity</t>
   </si>
@@ -79,15 +79,66 @@
     <t>Elevated</t>
   </si>
   <si>
+    <t>Likely</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Tampering</t>
+  </si>
+  <si>
+    <t>Development</t>
+  </si>
+  <si>
+    <t>CWE-79</t>
+  </si>
+  <si>
+    <t>Cross-Site Scripting (XSS)</t>
+  </si>
+  <si>
+    <t>Google Meet Server</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Cross-Site Scripting (XSS) risk at Google Meet Server</t>
+  </si>
+  <si>
+    <t>XSS Prevention</t>
+  </si>
+  <si>
+    <t>Try to encode all values sent back to the browser and also handle DOM-manipulations in a safe way to avoid DOM-based XSS. When a third-party product is used instead of custom developed software, check if the product applies the proper mitigation and ensure a reasonable patch-level.</t>
+  </si>
+  <si>
+    <t>Are recommendations from the linked cheat sheet and referenced ASVS chapter applied?</t>
+  </si>
+  <si>
+    <t>cross-site-scripting@google-meet-server</t>
+  </si>
+  <si>
+    <t>Unchecked</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Auth Server</t>
+  </si>
+  <si>
+    <t>Cross-Site Scripting (XSS) risk at Auth Server</t>
+  </si>
+  <si>
+    <t>cross-site-scripting@auth-server</t>
+  </si>
+  <si>
     <t>Unlikely</t>
   </si>
   <si>
     <t>Very High</t>
   </si>
   <si>
-    <t>Tampering</t>
-  </si>
-  <si>
     <t>Operations</t>
   </si>
   <si>
@@ -97,9 +148,6 @@
     <t>Missing Cloud Hardening</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Missing Cloud Hardening risk at Public Internet</t>
   </si>
   <si>
@@ -109,34 +157,169 @@
     <t>Apply hardening of all cloud components and services, taking special care to follow the individual risk descriptions (which depend on the cloud provider tags in the model). &lt;br&gt;&lt;br&gt;For &lt;b&gt;Amazon Web Services (AWS)&lt;/b&gt;: Follow the &lt;i&gt;CIS Benchmark for Amazon Web Services&lt;/i&gt; (see also the automated checks of cloud audit tools like &lt;i&gt;"PacBot", "CloudSploit", "CloudMapper", "ScoutSuite", or "Prowler AWS CIS Benchmark Tool"&lt;/i&gt;). &lt;br&gt;For EC2 and other servers running Amazon Linux, follow the &lt;i&gt;CIS Benchmark for Amazon Linux&lt;/i&gt; and switch to IMDSv2. &lt;br&gt;For S3 buckets follow the &lt;i&gt;Security Best Practices for Amazon S3&lt;/i&gt; at &lt;a href="https://docs.aws.amazon.com/AmazonS3/latest/dev/security-best-practices.html"&gt;https://docs.aws.amazon.com/AmazonS3/latest/dev/security-best-practices.html&lt;/a&gt; to avoid accidental leakage. &lt;br&gt;Also take a look at some of these tools: &lt;a href="https://github.com/toniblyx/my-arsenal-of-aws-security-tools"&gt;https://github.com/toniblyx/my-arsenal-of-aws-security-tools&lt;/a&gt; &lt;br&gt;&lt;br&gt;For &lt;b&gt;Microsoft Azure&lt;/b&gt;: Follow the &lt;i&gt;CIS Benchmark for Microsoft Azure&lt;/i&gt; (see also the automated checks of cloud audit tools like &lt;i&gt;"CloudSploit" or "ScoutSuite"&lt;/i&gt;).&lt;br&gt;&lt;br&gt;For &lt;b&gt;Google Cloud Platform&lt;/b&gt;: Follow the &lt;i&gt;CIS Benchmark for Google Cloud Computing Platform&lt;/i&gt; (see also the automated checks of cloud audit tools like &lt;i&gt;"CloudSploit" or "ScoutSuite"&lt;/i&gt;). &lt;br&gt;&lt;br&gt;For &lt;b&gt;Oracle Cloud Platform&lt;/b&gt;: Follow the hardening best practices (see also the automated checks of cloud audit tools like &lt;i&gt;"CloudSploit"&lt;/i&gt;).</t>
   </si>
   <si>
-    <t>Are recommendations from the linked cheat sheet and referenced ASVS chapter applied?</t>
-  </si>
-  <si>
     <t>missing-cloud-hardening@public-internet</t>
   </si>
   <si>
-    <t>Unchecked</t>
-  </si>
-  <si>
-    <t>Medium</t>
+    <t>CWE-16</t>
+  </si>
+  <si>
+    <t>Missing Hardening</t>
+  </si>
+  <si>
+    <t>Missing Hardening risk at Google Meet Server</t>
+  </si>
+  <si>
+    <t>System Hardening</t>
+  </si>
+  <si>
+    <t>Try to apply all hardening best practices (like CIS benchmarks, OWASP recommendations, vendor recommendations, DevSec Hardening Framework, DBSAT for Oracle databases, and others).</t>
+  </si>
+  <si>
+    <t>missing-hardening@google-meet-server</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Missing Hardening risk at Auth Server</t>
+  </si>
+  <si>
+    <t>missing-hardening@auth-server</t>
+  </si>
+  <si>
+    <t>CWE-912</t>
+  </si>
+  <si>
+    <t>Container Base Image Backdooring</t>
+  </si>
+  <si>
+    <t>Container Base Image Backdooring risk at Google Meet Server</t>
+  </si>
+  <si>
+    <t>Container Infrastructure Hardening</t>
+  </si>
+  <si>
+    <t>Apply hardening of all container infrastructures (see for example the &lt;i&gt;CIS-Benchmarks for Docker and Kubernetes&lt;/i&gt; and the &lt;i&gt;Docker Bench for Security&lt;/i&gt;). Use only trusted base images of the original vendors, verify digital signatures and apply image creation best practices. Also consider using Google's &lt;i&gt;Distroless&lt;/i&gt; base images or otherwise very small base images. Regularly execute container image scans with tools checking the layers for vulnerable components.</t>
+  </si>
+  <si>
+    <t>Are recommendations from the linked cheat sheet and referenced ASVS/CSVS applied?</t>
+  </si>
+  <si>
+    <t>container-baseimage-backdooring@google-meet-server</t>
+  </si>
+  <si>
+    <t>Very Likely</t>
+  </si>
+  <si>
+    <t>Spoofing</t>
+  </si>
+  <si>
+    <t>CWE-352</t>
+  </si>
+  <si>
+    <t>Cross-Site Request Forgery (CSRF)</t>
+  </si>
+  <si>
+    <t>User Authentication Access</t>
+  </si>
+  <si>
+    <t>Cross-Site Request Forgery (CSRF) risk at Auth Server via User Authentication Access from Google Meet Server</t>
+  </si>
+  <si>
+    <t>CSRF Prevention</t>
+  </si>
+  <si>
+    <t>Try to use anti-CSRF tokens ot the double-submit patterns (at least for logged-in requests). When your authentication scheme depends on cookies (like session or token cookies), consider marking them with the same-site flag. When a third-party product is used instead of custom developed software, check if the product applies the proper mitigation and ensure a reasonable patch-level.</t>
+  </si>
+  <si>
+    <t>cross-site-request-forgery@auth-server@google-meet-server&gt;user-authentication-access</t>
+  </si>
+  <si>
+    <t>Google Meet Traffic</t>
+  </si>
+  <si>
+    <t>Cross-Site Request Forgery (CSRF) risk at Google Meet Server via Google Meet Traffic from Load Balancer</t>
+  </si>
+  <si>
+    <t>cross-site-request-forgery@google-meet-server@load-balancer&gt;google-meet-traffic</t>
+  </si>
+  <si>
+    <t>Denial of Service</t>
+  </si>
+  <si>
+    <t>CWE-400</t>
+  </si>
+  <si>
+    <t>DoS-risky Access Across Trust-Boundary</t>
+  </si>
+  <si>
+    <t>Google Meet Client</t>
+  </si>
+  <si>
+    <t>Web Interface</t>
+  </si>
+  <si>
+    <t>Denial-of-Service risky access of Google Meet Client by Google Meet Server via Web Interface</t>
+  </si>
+  <si>
+    <t>Anti-DoS Measures</t>
+  </si>
+  <si>
+    <t>Apply anti-DoS techniques like throttling and/or per-client load blocking with quotas. Also for maintenance access routes consider applying a VPN instead of public reachable interfaces. Generally applying redundancy on the targeted technical asset reduces the risk of DoS.</t>
+  </si>
+  <si>
+    <t>dos-risky-access-across-trust-boundary@google-meet-client@google-meet-server@google-meet-server&gt;web-interface</t>
+  </si>
+  <si>
+    <t>Elevation of Privilege</t>
+  </si>
+  <si>
+    <t>Architecture</t>
+  </si>
+  <si>
+    <t>CWE-284</t>
+  </si>
+  <si>
+    <t>Missing Identity Propagation</t>
+  </si>
+  <si>
+    <t>Missing Enduser Identity Propagation over communication link Google Meet Traffic from Load Balancer to Google Meet Server</t>
+  </si>
+  <si>
+    <t>Identity Propagation and Resource-based Authorization</t>
+  </si>
+  <si>
+    <t>When processing requests for endusers if possible authorize in the backend against the propagated identity of the enduser. This can be achieved in passing JWTs or similar tokens and checking them in the backend services. For DevOps usages apply at least a technical-user authorization.</t>
+  </si>
+  <si>
+    <t>missing-identity-propagation@load-balancer&gt;google-meet-traffic@load-balancer@google-meet-server</t>
+  </si>
+  <si>
+    <t>Missing Identity Provider Isolation</t>
+  </si>
+  <si>
+    <t>Missing Identity Provider Isolation to further encapsulate and protect identity-related asset Auth Server against unrelated lower protected assets in the same network segment, which might be easier to compromise by attackers</t>
+  </si>
+  <si>
+    <t>Network Segmentation</t>
+  </si>
+  <si>
+    <t>Apply a network segmentation trust-boundary around the highly sensitive identity provider assets and their identity datastores.</t>
+  </si>
+  <si>
+    <t>missing-identity-provider-isolation@auth-server</t>
   </si>
   <si>
     <t>Information Disclosure</t>
   </si>
   <si>
-    <t>Architecture</t>
-  </si>
-  <si>
     <t>CWE-522</t>
   </si>
   <si>
     <t>Missing Vault (Secret Storage)</t>
   </si>
   <si>
-    <t>Web Application</t>
-  </si>
-  <si>
-    <t>Missing Vault (Secret Storage) in the threat model (referencing asset Web Application as an example)</t>
+    <t>Missing Vault (Secret Storage) in the threat model (referencing asset Google Meet Client as an example)</t>
   </si>
   <si>
     <t>Vault (Secret Storage)</t>
@@ -148,46 +331,100 @@
     <t>Is a Vault (Secret Storage) in place?</t>
   </si>
   <si>
-    <t>missing-vault@web-app</t>
-  </si>
-  <si>
-    <t>Low</t>
-  </si>
-  <si>
-    <t>Elevation of Privilege</t>
-  </si>
-  <si>
-    <t>Unnecessary Data Asset</t>
-  </si>
-  <si>
-    <t>Unnecessary Data Asset named User Account Information</t>
+    <t>missing-vault@google-meet-client</t>
+  </si>
+  <si>
+    <t>Mixed Targets on Shared Runtime</t>
+  </si>
+  <si>
+    <t>Mixed Targets on Shared Runtime named Google Cloud Platform might enable attackers moving from one less valuable target to a more valuable one</t>
+  </si>
+  <si>
+    <t>Runtime Separation</t>
+  </si>
+  <si>
+    <t>Use separate runtime environments for running different target components or apply similar separation styles to prevent load- or breach-related problems originating from one more attacker-facing asset impacts also the other more critical rated backend/datastore assets.</t>
+  </si>
+  <si>
+    <t>mixed-targets-on-shared-runtime@gcp</t>
+  </si>
+  <si>
+    <t>CWE-918</t>
+  </si>
+  <si>
+    <t>Server-Side Request Forgery (SSRF)</t>
+  </si>
+  <si>
+    <t>Server-Side Request Forgery (SSRF) risk at Google Meet Server server-side web-requesting the target Auth Server via User Authentication Access</t>
+  </si>
+  <si>
+    <t>SSRF Prevention</t>
+  </si>
+  <si>
+    <t>Try to avoid constructing the outgoing target URL with caller controllable values. Alternatively use a mapping (whitelist) when accessing outgoing URLs instead of creating them including caller controllable values. When a third-party product is used instead of custom developed software, check if the product applies the proper mitigation and ensure a reasonable patch-level.</t>
+  </si>
+  <si>
+    <t>server-side-request-forgery@google-meet-server@auth-server@google-meet-server&gt;user-authentication-access</t>
+  </si>
+  <si>
+    <t>Server-Side Request Forgery (SSRF) risk at Google Meet Server server-side web-requesting the target Google Meet Client via Web Interface</t>
+  </si>
+  <si>
+    <t>server-side-request-forgery@google-meet-server@google-meet-client@google-meet-server&gt;web-interface</t>
+  </si>
+  <si>
+    <t>CWE-319</t>
+  </si>
+  <si>
+    <t>Unencrypted Communication</t>
+  </si>
+  <si>
+    <t>Load Balancer</t>
+  </si>
+  <si>
+    <t>Unencrypted Communication named Google Meet Traffic between Load Balancer and Google Meet Server transferring authentication data (like credentials, token, session-id, etc.)</t>
+  </si>
+  <si>
+    <t>Encryption of Communication Links</t>
+  </si>
+  <si>
+    <t>Apply transport layer encryption to the communication link.</t>
+  </si>
+  <si>
+    <t>unencrypted-communication@load-balancer&gt;google-meet-traffic@load-balancer@google-meet-server</t>
+  </si>
+  <si>
+    <t>Unnecessary Data Transfer</t>
+  </si>
+  <si>
+    <t>Unnecessary Data Transfer of User Account Information data at Google Meet Client from/to Google Meet Server</t>
   </si>
   <si>
     <t>Attack Surface Reduction</t>
   </si>
   <si>
-    <t>Try to avoid having data assets that are not required/used.</t>
-  </si>
-  <si>
-    <t>unnecessary-data-asset@user-accounts</t>
-  </si>
-  <si>
-    <t>Unnecessary Data Asset named Video Meeting Data</t>
-  </si>
-  <si>
-    <t>unnecessary-data-asset@meeting-data</t>
+    <t>Try to avoid sending or receiving sensitive data assets which are not required (i.e. neither processed or stored) by the involved technical asset.</t>
+  </si>
+  <si>
+    <t>unnecessary-data-transfer@user-accounts@google-meet-client@google-meet-server</t>
+  </si>
+  <si>
+    <t>Unnecessary Data Transfer of Video Meeting Data data at Google Meet Client from/to Google Meet Server</t>
+  </si>
+  <si>
+    <t>unnecessary-data-transfer@meeting-data@google-meet-client@google-meet-server</t>
   </si>
   <si>
     <t>Unnecessary Technical Asset</t>
   </si>
   <si>
-    <t>Unnecessary Technical Asset named Web Application</t>
+    <t>Unnecessary Technical Asset named Google Meet Client</t>
   </si>
   <si>
     <t>Try to avoid using technical assets that do not process or store anything.</t>
   </si>
   <si>
-    <t>unnecessary-technical-asset@web-app</t>
+    <t>unnecessary-technical-asset@google-meet-client</t>
   </si>
 </sst>
 </file>
@@ -809,28 +1046,28 @@
         <v>27</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J2" s="18">
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="K2" s="19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L2" s="22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M2" s="22" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N2" s="22" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O2" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Q2" s="19"/>
       <c r="R2" s="17"/>
@@ -838,53 +1075,53 @@
       <c r="T2" s="16"/>
     </row>
     <row r="3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="18">
+        <v>100</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O3" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3" s="10" t="s">
         <v>34</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3" s="18">
-        <v>1</v>
-      </c>
-      <c r="K3" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="L3" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="M3" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="N3" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="O3" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="P3" s="10" t="s">
-        <v>33</v>
       </c>
       <c r="Q3" s="19"/>
       <c r="R3" s="17"/>
@@ -892,53 +1129,53 @@
       <c r="T3" s="16"/>
     </row>
     <row r="4">
-      <c r="A4" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>27</v>
+      <c r="A4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="J4" s="18">
         <v>0</v>
       </c>
       <c r="K4" s="19" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="L4" s="22" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="M4" s="22" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="N4" s="22" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O4" s="20" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="P4" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Q4" s="19"/>
       <c r="R4" s="17"/>
@@ -946,53 +1183,53 @@
       <c r="T4" s="16"/>
     </row>
     <row r="5">
-      <c r="A5" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="10" t="s">
+      <c r="A5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H5" s="9" t="s">
+      <c r="C5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>27</v>
+      <c r="I5" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="J5" s="18">
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="K5" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="L5" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="M5" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="L5" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="M5" s="22" t="s">
-        <v>50</v>
-      </c>
       <c r="N5" s="22" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O5" s="20" t="s">
         <v>53</v>
       </c>
       <c r="P5" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Q5" s="19"/>
       <c r="R5" s="17"/>
@@ -1000,58 +1237,814 @@
       <c r="T5" s="16"/>
     </row>
     <row r="6">
-      <c r="A6" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="10" t="s">
+      <c r="A6" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" s="10" t="s">
+      <c r="C6" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>27</v>
+      <c r="I6" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="J6" s="18">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="K6" s="19" t="s">
         <v>55</v>
       </c>
       <c r="L6" s="22" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="M6" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="N6" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O6" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="N6" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="O6" s="20" t="s">
-        <v>57</v>
-      </c>
       <c r="P6" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Q6" s="19"/>
       <c r="R6" s="17"/>
       <c r="S6" s="17"/>
       <c r="T6" s="16"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="18">
+        <v>93</v>
+      </c>
+      <c r="K7" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="L7" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="M7" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="N7" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="O7" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="P7" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="17"/>
+      <c r="T7" s="16"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="J8" s="18">
+        <v>100</v>
+      </c>
+      <c r="K8" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="L8" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="M8" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="N8" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O8" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="P8" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="17"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="16"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J9" s="18">
+        <v>93</v>
+      </c>
+      <c r="K9" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="L9" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="M9" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="N9" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O9" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="P9" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="17"/>
+      <c r="S9" s="17"/>
+      <c r="T9" s="16"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="J10" s="18">
+        <v>1</v>
+      </c>
+      <c r="K10" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="L10" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="M10" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="N10" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O10" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="P10" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="17"/>
+      <c r="S10" s="17"/>
+      <c r="T10" s="16"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J11" s="18">
+        <v>93</v>
+      </c>
+      <c r="K11" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="L11" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="M11" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="N11" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O11" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="P11" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="17"/>
+      <c r="S11" s="17"/>
+      <c r="T11" s="16"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" s="18">
+        <v>100</v>
+      </c>
+      <c r="K12" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="L12" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="M12" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="N12" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O12" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="P12" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="17"/>
+      <c r="S12" s="17"/>
+      <c r="T12" s="16"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J13" s="18">
+        <v>1</v>
+      </c>
+      <c r="K13" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="L13" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="M13" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="N13" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="O13" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="P13" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q13" s="19"/>
+      <c r="R13" s="17"/>
+      <c r="S13" s="17"/>
+      <c r="T13" s="16"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" s="18">
+        <v>0</v>
+      </c>
+      <c r="K14" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="L14" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="M14" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="N14" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O14" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="P14" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q14" s="19"/>
+      <c r="R14" s="17"/>
+      <c r="S14" s="17"/>
+      <c r="T14" s="16"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="J15" s="18">
+        <v>93</v>
+      </c>
+      <c r="K15" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="L15" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="M15" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="N15" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O15" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="P15" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q15" s="19"/>
+      <c r="R15" s="17"/>
+      <c r="S15" s="17"/>
+      <c r="T15" s="16"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="J16" s="18">
+        <v>93</v>
+      </c>
+      <c r="K16" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="L16" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="M16" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="N16" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O16" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="P16" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q16" s="19"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
+      <c r="T16" s="16"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J17" s="18">
+        <v>7</v>
+      </c>
+      <c r="K17" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="L17" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="M17" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="N17" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O17" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="P17" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="17"/>
+      <c r="S17" s="17"/>
+      <c r="T17" s="16"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J18" s="18">
+        <v>1</v>
+      </c>
+      <c r="K18" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="L18" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="M18" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="N18" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O18" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="P18" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q18" s="19"/>
+      <c r="R18" s="17"/>
+      <c r="S18" s="17"/>
+      <c r="T18" s="16"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J19" s="18">
+        <v>1</v>
+      </c>
+      <c r="K19" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="L19" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="M19" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="N19" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O19" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="P19" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q19" s="19"/>
+      <c r="R19" s="17"/>
+      <c r="S19" s="17"/>
+      <c r="T19" s="16"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J20" s="18">
+        <v>1</v>
+      </c>
+      <c r="K20" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="L20" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="M20" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="N20" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O20" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="P20" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q20" s="19"/>
+      <c r="R20" s="17"/>
+      <c r="S20" s="17"/>
+      <c r="T20" s="16"/>
     </row>
   </sheetData>
   <pageSetup orientation="landscape" paperSize="9"/>

</xml_diff>